<commit_message>
lan 13 , check va cham boss voi kiem va sung, render anh victory
</commit_message>
<xml_diff>
--- a/MAP/map04.xlsx
+++ b/MAP/map04.xlsx
@@ -1,59 +1,401 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\bat_dau_game\MAP\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965C7672-AE90-434F-88F7-B340B8BC1AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₫&quot;_-;\-* #,##0.00\ &quot;₫&quot;_-;_-* &quot;-&quot;??\ &quot;₫&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0\ &quot;₫&quot;_-;\-* #,##0\ &quot;₫&quot;_-;_-* &quot;-&quot;\ &quot;₫&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Calibri"/>
       <charset val="163"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="8"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -61,23 +403,355 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="7" tint="-0.499984740745262"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.349986266670736"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="-0.249946592608417"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.599963377788629"/>
         </patternFill>
       </fill>
     </dxf>
@@ -91,63 +765,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="7" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -156,9 +774,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -416,30 +1031,31 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:EJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BN25" workbookViewId="0">
-      <selection activeCell="CX50" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BL13" workbookViewId="0">
+      <selection activeCell="DU48" sqref="DU48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="2.62857142857143" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="3.625"/>
-    <col min="16" max="16" width="3.625"/>
-    <col min="38" max="38" width="3.625"/>
-    <col min="44" max="44" width="2.875" customWidth="1"/>
-    <col min="56" max="56" width="3.625"/>
-    <col min="66" max="66" width="2.875" customWidth="1"/>
-    <col min="73" max="73" width="2.875" customWidth="1"/>
-    <col min="76" max="76" width="2.875" customWidth="1"/>
-    <col min="85" max="85" width="2.875" customWidth="1"/>
-    <col min="100" max="100" width="3.625"/>
+    <col min="6" max="6" width="3.62857142857143"/>
+    <col min="16" max="16" width="3.62857142857143"/>
+    <col min="38" max="38" width="3.62857142857143"/>
+    <col min="44" max="44" width="2.87619047619048" customWidth="1"/>
+    <col min="56" max="56" width="3.62857142857143"/>
+    <col min="66" max="66" width="2.87619047619048" customWidth="1"/>
+    <col min="73" max="73" width="2.87619047619048" customWidth="1"/>
+    <col min="76" max="76" width="2.87619047619048" customWidth="1"/>
+    <col min="85" max="85" width="2.87619047619048" customWidth="1"/>
+    <col min="100" max="100" width="3.62857142857143"/>
+    <col min="113" max="113" width="3.57142857142857"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:140">
@@ -1363,16 +1979,16 @@
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -4066,7 +4682,7 @@
         <v>0</v>
       </c>
       <c r="CE9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CF9">
         <v>0</v>
@@ -4075,7 +4691,7 @@
         <v>0</v>
       </c>
       <c r="CH9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CI9">
         <v>0</v>
@@ -4084,7 +4700,7 @@
         <v>0</v>
       </c>
       <c r="CK9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CL9">
         <v>0</v>
@@ -4960,7 +5576,7 @@
       <c r="CU11">
         <v>0</v>
       </c>
-      <c r="CV11" s="2">
+      <c r="CV11" s="1">
         <v>22</v>
       </c>
       <c r="CW11">
@@ -5382,7 +5998,7 @@
       <c r="CU12">
         <v>0</v>
       </c>
-      <c r="CV12" s="1">
+      <c r="CV12" s="2">
         <v>0</v>
       </c>
       <c r="CW12">
@@ -5804,7 +6420,7 @@
       <c r="CU13">
         <v>0</v>
       </c>
-      <c r="CV13" s="1">
+      <c r="CV13" s="2">
         <v>0</v>
       </c>
       <c r="CW13">
@@ -6008,7 +6624,7 @@
         <v>7</v>
       </c>
       <c r="AA14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB14">
         <v>0</v>
@@ -7041,7 +7657,7 @@
         <v>1</v>
       </c>
       <c r="CL16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CM16">
         <v>0</v>
@@ -9211,37 +9827,37 @@
         <v>0</v>
       </c>
       <c r="DF21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DG21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DH21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DI21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DJ21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DK21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DL21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DM21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DN21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DO21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DP21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DQ21">
         <v>0</v>
@@ -10124,7 +10740,7 @@
         <v>1</v>
       </c>
       <c r="EC23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="ED23">
         <v>0</v>
@@ -12081,7 +12697,7 @@
         <v>0</v>
       </c>
       <c r="CD28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CE28">
         <v>2</v>
@@ -13910,28 +14526,28 @@
         <v>0</v>
       </c>
       <c r="DY32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="DZ32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EA32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EB32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EC32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="ED32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EE32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EF32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="EG32">
         <v>9</v>
@@ -14733,7 +15349,7 @@
         <v>0</v>
       </c>
       <c r="DR34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="DS34">
         <v>6</v>
@@ -15128,7 +15744,7 @@
         <v>0</v>
       </c>
       <c r="DI35">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="DJ35">
         <v>0</v>
@@ -15792,7 +16408,7 @@
         <v>0</v>
       </c>
       <c r="BA37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BB37">
         <v>4</v>
@@ -16780,58 +17396,58 @@
         <v>8</v>
       </c>
       <c r="CW39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="CX39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="CY39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="CZ39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DA39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DB39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DC39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DD39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DE39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DF39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DG39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DH39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DI39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DJ39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DK39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DL39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DM39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DN39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="DO39">
         <v>0</v>
@@ -19434,46 +20050,47 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="BQ24">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>23</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BL29">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+  <conditionalFormatting sqref="$A1:$XFD1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>24</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>13</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
       <formula>1</formula>
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>